<commit_message>
checked comaptibility against ff3c_v127, it found to be hard to compatible :sad:
</commit_message>
<xml_diff>
--- a/docs/development/changes-by-address-range.xlsx
+++ b/docs/development/changes-by-address-range.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="169">
   <si>
     <t xml:space="preserve">[start,end)  </t>
   </si>
@@ -579,6 +579,19 @@
   </si>
   <si>
     <t>069b79-06a000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0.8.0
+ff3c_v127</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>!</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -685,7 +698,43 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -757,24 +806,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -876,17 +907,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル1" displayName="テーブル1" ref="A1:H83" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:H83"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="[start,end)  " dataDxfId="9"/>
-    <tableColumn id="2" name="usage " dataDxfId="6"/>
-    <tableColumn id="4" name="uff3_1.14_x000a_plain" dataDxfId="5"/>
-    <tableColumn id="5" name="0.7.9d_x000a_plain" dataDxfId="3"/>
-    <tableColumn id="6" name="0.7.9d_x000a_ uff3_1.14" dataDxfId="2"/>
-    <tableColumn id="7" name="0.7.9d_x000a_0.8.0beta1" dataDxfId="1"/>
-    <tableColumn id="8" name="0.7.9d_x000a_0.8.0-window-only" dataDxfId="0"/>
-    <tableColumn id="3" name=" description" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル1" displayName="テーブル1" ref="A1:I83" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I83"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="[start,end)  " dataDxfId="8"/>
+    <tableColumn id="2" name="usage " dataDxfId="7"/>
+    <tableColumn id="4" name="uff3_1.14_x000a_plain" dataDxfId="6"/>
+    <tableColumn id="5" name="0.7.9d_x000a_plain" dataDxfId="5"/>
+    <tableColumn id="6" name="0.7.9d_x000a_ uff3_1.14" dataDxfId="4"/>
+    <tableColumn id="7" name="0.7.9d_x000a_0.8.0beta1" dataDxfId="3"/>
+    <tableColumn id="8" name="0.7.9d_x000a_0.8.0-window-only" dataDxfId="2"/>
+    <tableColumn id="9" name="0.8.0_x000a_ff3c_v127" dataDxfId="0"/>
+    <tableColumn id="3" name=" description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1155,13 +1187,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H69" sqref="H69"/>
+      <selection pane="bottomRight" activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1169,12 +1201,12 @@
     <col min="1" max="1" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="5.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="5.25" style="3" customWidth="1"/>
-    <col min="8" max="8" width="88.125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="1"/>
+    <col min="5" max="8" width="5.25" style="3" customWidth="1"/>
+    <col min="9" max="9" width="88.125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="83.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="83.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1196,13 +1228,16 @@
       <c r="G1" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1224,13 +1259,16 @@
       <c r="G2" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1252,13 +1290,16 @@
       <c r="G3" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1280,13 +1321,16 @@
       <c r="G4" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1308,13 +1352,16 @@
       <c r="G5" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1336,13 +1383,16 @@
       <c r="G6" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1364,10 +1414,13 @@
       <c r="G7" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="H7" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1389,13 +1442,16 @@
       <c r="G8" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1417,13 +1473,16 @@
       <c r="G9" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1445,13 +1504,16 @@
       <c r="G10" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1473,13 +1535,16 @@
       <c r="G11" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1501,13 +1566,16 @@
       <c r="G12" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1529,10 +1597,13 @@
       <c r="G13" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="H13" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1554,13 +1625,16 @@
       <c r="G14" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1582,13 +1656,16 @@
       <c r="G15" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.15">
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1610,13 +1687,16 @@
       <c r="G16" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1638,13 +1718,16 @@
       <c r="G17" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -1666,10 +1749,13 @@
       <c r="G18" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="H18" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1691,13 +1777,16 @@
       <c r="G19" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1719,13 +1808,16 @@
       <c r="G20" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1747,13 +1839,16 @@
       <c r="G21" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1775,13 +1870,16 @@
       <c r="G22" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1803,13 +1901,16 @@
       <c r="G23" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -1831,13 +1932,16 @@
       <c r="G24" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -1859,13 +1963,16 @@
       <c r="G25" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -1887,13 +1994,16 @@
       <c r="G26" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -1915,13 +2025,16 @@
       <c r="G27" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -1943,13 +2056,16 @@
       <c r="G28" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -1971,13 +2087,16 @@
       <c r="G29" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -1999,13 +2118,16 @@
       <c r="G30" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -2027,13 +2149,16 @@
       <c r="G31" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -2055,13 +2180,16 @@
       <c r="G32" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -2083,13 +2211,16 @@
       <c r="G33" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -2111,13 +2242,16 @@
       <c r="G34" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I34" s="1"/>
       <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -2139,13 +2273,16 @@
       <c r="G35" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="I35" s="1"/>
       <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -2167,13 +2304,16 @@
       <c r="G36" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I36" s="1"/>
       <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -2195,13 +2335,16 @@
       <c r="G37" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I37" s="1"/>
       <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -2223,13 +2366,16 @@
       <c r="G38" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I38" s="1"/>
       <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -2251,13 +2397,16 @@
       <c r="G39" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -2279,13 +2428,16 @@
       <c r="G40" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -2307,13 +2459,16 @@
       <c r="G41" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I41" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -2335,13 +2490,16 @@
       <c r="G42" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I42" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -2363,13 +2521,16 @@
       <c r="G43" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H43" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I43" s="1"/>
       <c r="J43" s="1"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -2391,13 +2552,16 @@
       <c r="G44" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I44" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>154</v>
       </c>
@@ -2419,13 +2583,16 @@
       <c r="G45" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H45" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I45" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="I45" s="1"/>
       <c r="J45" s="1"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -2447,13 +2614,16 @@
       <c r="G46" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I46" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="I46" s="1"/>
       <c r="J46" s="1"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -2475,13 +2645,16 @@
       <c r="G47" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H47" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I47" s="1"/>
       <c r="J47" s="1"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -2503,13 +2676,16 @@
       <c r="G48" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I48" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -2531,13 +2707,16 @@
       <c r="G49" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="I49" s="1"/>
       <c r="J49" s="1"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -2559,13 +2738,16 @@
       <c r="G50" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="H50" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I50" s="1"/>
       <c r="J50" s="1"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -2587,13 +2769,16 @@
       <c r="G51" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H51" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
@@ -2615,13 +2800,16 @@
       <c r="G52" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="H52" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I52" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I52" s="1"/>
       <c r="J52" s="1"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
@@ -2643,13 +2831,16 @@
       <c r="G53" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H53" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I53" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="I53" s="1"/>
       <c r="J53" s="1"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
@@ -2671,13 +2862,16 @@
       <c r="G54" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="H54" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I54" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I54" s="1"/>
       <c r="J54" s="1"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
@@ -2699,13 +2893,16 @@
       <c r="G55" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="H55" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I55" s="1"/>
       <c r="J55" s="1"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
@@ -2727,13 +2924,16 @@
       <c r="G56" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H56" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I56" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I56" s="1"/>
       <c r="J56" s="1"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
@@ -2755,13 +2955,16 @@
       <c r="G57" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I57" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I57" s="1"/>
       <c r="J57" s="1"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
@@ -2783,13 +2986,16 @@
       <c r="G58" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="H58" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I58" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I58" s="1"/>
       <c r="J58" s="1"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K58" s="1"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>78</v>
       </c>
@@ -2811,13 +3017,16 @@
       <c r="G59" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I59" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I59" s="1"/>
       <c r="J59" s="1"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>76</v>
       </c>
@@ -2839,13 +3048,16 @@
       <c r="G60" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="H60" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I60" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I60" s="1"/>
       <c r="J60" s="1"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K60" s="1"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>84</v>
       </c>
@@ -2867,13 +3079,16 @@
       <c r="G61" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H61" s="2" t="s">
+      <c r="H61" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I61" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I61" s="1"/>
       <c r="J61" s="1"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>85</v>
       </c>
@@ -2895,13 +3110,16 @@
       <c r="G62" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H62" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I62" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I62" s="1"/>
       <c r="J62" s="1"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>86</v>
       </c>
@@ -2923,13 +3141,16 @@
       <c r="G63" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="H63" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I63" s="1"/>
       <c r="J63" s="1"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>162</v>
       </c>
@@ -2951,13 +3172,16 @@
       <c r="G64" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="H64" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I64" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I64" s="1"/>
       <c r="J64" s="1"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K64" s="1"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>164</v>
       </c>
@@ -2979,13 +3203,16 @@
       <c r="G65" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="H65" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I65" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="I65" s="1"/>
       <c r="J65" s="1"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K65" s="1"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>165</v>
       </c>
@@ -2993,10 +3220,13 @@
         <v>75</v>
       </c>
       <c r="E66" s="9"/>
-      <c r="I66" s="1"/>
+      <c r="H66" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="J66" s="1"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K66" s="1"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>87</v>
       </c>
@@ -3018,13 +3248,16 @@
       <c r="G67" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="H67" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I67" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I67" s="1"/>
       <c r="J67" s="1"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K67" s="1"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>63</v>
       </c>
@@ -3046,13 +3279,16 @@
       <c r="G68" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H68" s="2" t="s">
+      <c r="H68" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I68" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I68" s="1"/>
       <c r="J68" s="1"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K68" s="1"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>64</v>
       </c>
@@ -3074,13 +3310,16 @@
       <c r="G69" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="H69" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I69" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I69" s="1"/>
       <c r="J69" s="1"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K69" s="1"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>65</v>
       </c>
@@ -3102,13 +3341,16 @@
       <c r="G70" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="H70" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I70" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I70" s="1"/>
       <c r="J70" s="1"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K70" s="1"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>66</v>
       </c>
@@ -3130,10 +3372,13 @@
       <c r="G71" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I71" s="1"/>
+      <c r="H71" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="J71" s="1"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K71" s="1"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>67</v>
       </c>
@@ -3155,13 +3400,16 @@
       <c r="G72" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="H72" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I72" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I72" s="1"/>
       <c r="J72" s="1"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K72" s="1"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>68</v>
       </c>
@@ -3183,10 +3431,13 @@
       <c r="G73" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I73" s="1"/>
+      <c r="H73" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="J73" s="1"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K73" s="1"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>69</v>
       </c>
@@ -3208,13 +3459,16 @@
       <c r="G74" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="H74" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I74" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I74" s="1"/>
       <c r="J74" s="1"/>
-    </row>
-    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.15">
+      <c r="K74" s="1"/>
+    </row>
+    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>70</v>
       </c>
@@ -3236,13 +3490,16 @@
       <c r="G75" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="H75" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I75" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I75" s="1"/>
       <c r="J75" s="1"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K75" s="1"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>71</v>
       </c>
@@ -3264,13 +3521,16 @@
       <c r="G76" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="H76" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I76" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="I76" s="1"/>
       <c r="J76" s="1"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K76" s="1"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
         <v>72</v>
       </c>
@@ -3292,13 +3552,16 @@
       <c r="G77" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="H77" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I77" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I77" s="1"/>
       <c r="J77" s="1"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K77" s="1"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
         <v>73</v>
       </c>
@@ -3320,13 +3583,16 @@
       <c r="G78" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H78" s="5" t="s">
+      <c r="H78" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I78" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="I78" s="1"/>
       <c r="J78" s="1"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K78" s="1"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
         <v>79</v>
       </c>
@@ -3348,13 +3614,16 @@
       <c r="G79" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="H79" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I79" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I79" s="1"/>
       <c r="J79" s="1"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K79" s="1"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
         <v>80</v>
       </c>
@@ -3376,13 +3645,16 @@
       <c r="G80" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="H80" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I80" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I80" s="1"/>
       <c r="J80" s="1"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K80" s="1"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>81</v>
       </c>
@@ -3404,13 +3676,16 @@
       <c r="G81" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="H81" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I81" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I81" s="1"/>
       <c r="J81" s="1"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K81" s="1"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
@@ -3432,11 +3707,14 @@
       <c r="G82" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H82" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I82" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>83</v>
       </c>
@@ -3458,7 +3736,10 @@
       <c r="G83" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="H83" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I83" s="2" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>